<commit_message>
finished batch meter read
</commit_message>
<xml_diff>
--- a/doc/水表功能列表.xlsx
+++ b/doc/水表功能列表.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BFC59-A9E9-4DEC-A820-F97924E7B9E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3492" yWindow="720" windowWidth="17280" windowHeight="10584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="720" windowWidth="17280" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="223">
   <si>
     <t>表端</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -707,6 +706,192 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>户号：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>门牌号：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机：</t>
+  </si>
+  <si>
+    <t>地址：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表状态：已抄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表时间：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表读数：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表状态：（告警/阀门状态）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">电池电压：   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表方式：手持机/集中器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开阀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关阀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清异常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;楼栋抄表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;自动抄表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表进度 n/m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按楼栋抄表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;抄表统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;抄表统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>户表查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;户表查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;户表查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;户表信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>户名：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信号强度：(上行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抄表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回       户表命令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">返回   &lt;轮抄中&gt;  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.按表号显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.按户名显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.按户号显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.按门牌号显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小区选择：[全部] [单个]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼栋选择：[全部] [单个]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小区：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼栋：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回              确定</t>
+  </si>
+  <si>
+    <t>返回              确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回              确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回           户表信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;已抄/未抄列表    n/m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;已抄/未抄列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>户表命令     1/4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回           确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>&lt;&lt;小区列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -715,169 +900,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>户号：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>门牌号：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机：</t>
-  </si>
-  <si>
-    <t>地址：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表状态：已抄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表时间：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表读数：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表状态：（告警/阀门状态）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">电池电压：   </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表方式：手持机/集中器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开阀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关阀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>清异常</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回 &lt;等待输入&gt; 统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;楼栋抄表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;已抄/未抄列表    n/m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;自动抄表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表进度 n/m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>按楼栋抄表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;抄表统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;抄表统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>户表查询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;户表查询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;户表查询</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;户表信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>户名：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>信号强度：(上行)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抄表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回       户表命令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">返回   &lt;轮抄中&gt;  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  已抄列表显示方式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.按表号显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.按户名显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.按户号显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.按门牌号显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">      户表命令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小区：[全部] [单个]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>楼栋：[全部] [单个]</t>
+    <t xml:space="preserve"> 清空中… --&gt; 已清空！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 重置中… --&gt; 已重置！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1043,7 +1077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1061,7 +1095,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1085,13 +1118,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1099,7 +1132,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1138,13 +1171,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1057275</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>95252</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1152,7 +1185,7 @@
         <xdr:cNvPr id="5" name="直接箭头连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1191,13 +1224,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1205,7 +1238,7 @@
         <xdr:cNvPr id="7" name="直接箭头连接符 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1244,13 +1277,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1258,7 +1291,7 @@
         <xdr:cNvPr id="12" name="直接箭头连接符 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1297,13 +1330,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1311,7 +1344,7 @@
         <xdr:cNvPr id="14" name="直接箭头连接符 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,13 +1383,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>114302</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1364,7 +1397,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1403,13 +1436,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>57152</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1417,7 +1450,7 @@
         <xdr:cNvPr id="25" name="直接箭头连接符 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1456,13 +1489,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>114303</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1470,7 +1503,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1509,13 +1542,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1523,7 +1556,7 @@
         <xdr:cNvPr id="32" name="直接箭头连接符 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,13 +1595,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1576,7 +1609,7 @@
         <xdr:cNvPr id="34" name="直接箭头连接符 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1615,13 +1648,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1629,7 +1662,7 @@
         <xdr:cNvPr id="38" name="直接箭头连接符 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1668,13 +1701,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>123828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1682,7 +1715,7 @@
         <xdr:cNvPr id="39" name="直接箭头连接符 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1721,13 +1754,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1735,7 +1768,7 @@
         <xdr:cNvPr id="58" name="直接箭头连接符 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1774,13 +1807,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1788,7 +1821,7 @@
         <xdr:cNvPr id="59" name="直接箭头连接符 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1827,13 +1860,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>114302</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1841,7 +1874,7 @@
         <xdr:cNvPr id="60" name="直接箭头连接符 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1880,13 +1913,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1894,7 +1927,7 @@
         <xdr:cNvPr id="66" name="直接箭头连接符 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1933,13 +1966,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1947,7 +1980,7 @@
         <xdr:cNvPr id="2" name="箭头: 右 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1993,21 +2026,21 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="19" name="直接箭头连接符 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2015,8 +2048,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4800600" y="285750"/>
-          <a:ext cx="1847850" cy="1333500"/>
+          <a:off x="4800600" y="1009650"/>
+          <a:ext cx="1905000" cy="1162051"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2046,13 +2079,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>85727</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2060,7 +2093,7 @@
         <xdr:cNvPr id="20" name="直接箭头连接符 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2099,13 +2132,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1038225</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2113,7 +2146,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2152,13 +2185,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>57152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2166,7 +2199,7 @@
         <xdr:cNvPr id="26" name="直接箭头连接符 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2203,23 +2236,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104778</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57154</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="24" name="直接箭头连接符 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2227,8 +2260,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7905750" y="276225"/>
-          <a:ext cx="238125" cy="3"/>
+          <a:off x="7886700" y="304800"/>
+          <a:ext cx="428625" cy="609604"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2258,13 +2291,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2272,7 +2305,7 @@
         <xdr:cNvPr id="33" name="直接箭头连接符 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2311,13 +2344,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2325,7 +2358,7 @@
         <xdr:cNvPr id="35" name="直接箭头连接符 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2363,84 +2396,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="45" name="直接箭头连接符 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9467850" y="609600"/>
-          <a:ext cx="495300" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="直接箭头连接符 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9467850" y="266700"/>
-          <a:ext cx="495300" cy="9525"/>
+        <a:xfrm>
+          <a:off x="9601200" y="666750"/>
+          <a:ext cx="409575" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2470,13 +2450,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>1438275</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2484,7 +2464,7 @@
         <xdr:cNvPr id="53" name="直接箭头连接符 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2492,8 +2472,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="13373100" y="809625"/>
-          <a:ext cx="2600325" cy="1381126"/>
+          <a:off x="13325475" y="1571625"/>
+          <a:ext cx="2752725" cy="619126"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2522,67 +2502,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>1485900</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85728</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="直接箭头连接符 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="11563350" y="600075"/>
-          <a:ext cx="238125" cy="3"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2590,7 +2517,7 @@
         <xdr:cNvPr id="56" name="直接箭头连接符 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2598,8 +2525,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10972800" y="238126"/>
-          <a:ext cx="876300" cy="2552699"/>
+          <a:off x="11068050" y="981075"/>
+          <a:ext cx="781050" cy="2495550"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2629,13 +2556,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2643,7 +2570,7 @@
         <xdr:cNvPr id="61" name="直接箭头连接符 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2682,13 +2609,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2696,7 +2623,7 @@
         <xdr:cNvPr id="62" name="直接箭头连接符 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2735,13 +2662,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2749,7 +2676,7 @@
         <xdr:cNvPr id="63" name="直接箭头连接符 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2787,22 +2714,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="69" name="直接箭头连接符 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2810,8 +2737,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="12773025" y="2286000"/>
-          <a:ext cx="4105275" cy="2676525"/>
+          <a:off x="12582525" y="2257425"/>
+          <a:ext cx="4733925" cy="2762250"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2841,13 +2768,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>1581150</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2855,7 +2782,7 @@
         <xdr:cNvPr id="83" name="直接箭头连接符 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2865,6 +2792,271 @@
         <a:xfrm flipV="1">
           <a:off x="15440025" y="4962525"/>
           <a:ext cx="628650" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="直接箭头连接符 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9429750" y="2181225"/>
+          <a:ext cx="495300" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142877</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="直接箭头连接符 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11410950" y="657225"/>
+          <a:ext cx="409575" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="直接箭头连接符 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9686925" y="495300"/>
+          <a:ext cx="361950" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66680</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="直接箭头连接符 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7829550" y="323850"/>
+          <a:ext cx="4124325" cy="771530"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104782</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="直接箭头连接符 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7848600" y="314325"/>
+          <a:ext cx="6038850" cy="990607"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2936,7 +3128,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2969,26 +3161,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3021,23 +3196,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3213,1448 +3371,1449 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:W78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:W82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" customWidth="1"/>
-    <col min="4" max="4" width="4.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="3.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="4.109375" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="3.77734375" customWidth="1"/>
-    <col min="15" max="15" width="19.21875" customWidth="1"/>
-    <col min="16" max="16" width="3.33203125" customWidth="1"/>
-    <col min="17" max="17" width="19.88671875" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" customWidth="1"/>
-    <col min="19" max="19" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="3.125" customWidth="1"/>
+    <col min="4" max="4" width="4.125" customWidth="1"/>
+    <col min="5" max="5" width="13.75" customWidth="1"/>
+    <col min="6" max="6" width="4.25" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="3.125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="4.125" customWidth="1"/>
+    <col min="11" max="11" width="13.375" customWidth="1"/>
+    <col min="12" max="12" width="3.625" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="3.75" customWidth="1"/>
+    <col min="15" max="15" width="19.25" customWidth="1"/>
+    <col min="16" max="16" width="3.375" customWidth="1"/>
+    <col min="17" max="17" width="19.875" customWidth="1"/>
+    <col min="18" max="18" width="3.875" customWidth="1"/>
+    <col min="19" max="19" width="19.875" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="25.44140625" customWidth="1"/>
-    <col min="22" max="22" width="4.44140625" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
+    <col min="21" max="21" width="25.5" customWidth="1"/>
+    <col min="22" max="22" width="4.5" customWidth="1"/>
+    <col min="23" max="23" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O2" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="S2" t="s">
+        <v>221</v>
+      </c>
+      <c r="U2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O4" s="14"/>
+      <c r="Q4" s="14"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O5" s="14"/>
+      <c r="Q5" s="14"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H6">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I6" t="s">
         <v>133</v>
       </c>
-      <c r="L2">
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
-        <v>192</v>
-      </c>
-      <c r="O2" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H3">
+      <c r="M6" t="s">
+        <v>188</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I7" t="s">
         <v>62</v>
       </c>
-      <c r="L3">
+      <c r="L7">
         <v>2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H8">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I8" t="s">
         <v>136</v>
       </c>
-      <c r="L4">
+      <c r="L8">
         <v>3</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M8" t="s">
         <v>138</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="T4" s="5"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="W4" s="6"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="N8" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="Q8" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A9">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="H9">
         <v>4</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I9" t="s">
         <v>137</v>
       </c>
-      <c r="L5">
+      <c r="L9">
         <v>4</v>
       </c>
-      <c r="M5" t="s">
-        <v>197</v>
-      </c>
-      <c r="N5" s="7">
+      <c r="M9" t="s">
+        <v>193</v>
+      </c>
+      <c r="N9" s="7">
         <v>1</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="7" t="s">
+      <c r="Q9" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="7" t="s">
+      <c r="S9" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="V5" s="8"/>
-      <c r="W5" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>196</v>
-      </c>
-      <c r="N6" s="7">
-        <v>2</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="T6" s="8"/>
-      <c r="U6" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="V6" s="8"/>
-      <c r="W6" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N7" s="7">
-        <v>3</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="T7" s="8"/>
-      <c r="U7" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="V7" s="8"/>
-      <c r="W7" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="T8" s="8"/>
-      <c r="U8" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="V8" s="8"/>
-      <c r="W8" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>135</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>201</v>
       </c>
       <c r="T9" s="8"/>
       <c r="U9" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="V9" s="8"/>
-      <c r="W9" s="9"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="13" t="s">
-        <v>194</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>192</v>
+      </c>
+      <c r="N10" s="7">
+        <v>2</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="14"/>
       <c r="S10" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="T10" s="8"/>
       <c r="U10" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="V10" s="17"/>
-      <c r="W10" s="9"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O11" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="14" t="s">
-        <v>167</v>
-      </c>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" s="7">
+        <v>3</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q11" s="14"/>
       <c r="S11" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="T11" s="8"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="9"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O12" s="7" t="s">
+      <c r="U11" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>135</v>
+      </c>
+      <c r="N12" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="S12" s="7"/>
+      <c r="O12" s="12"/>
+      <c r="Q12" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>176</v>
+      </c>
       <c r="T12" s="8"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="9"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="S13" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="T13" s="11"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="12"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O14" s="7"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O15" s="7"/>
+      <c r="U12" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="W12" s="13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>134</v>
+      </c>
+      <c r="S13" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="T13" s="8"/>
+      <c r="U13" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="W13" s="14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="U14" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O15" s="7" t="s">
+        <v>206</v>
+      </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="T15" s="8"/>
+      <c r="U15" s="9"/>
+      <c r="W15" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O16" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="S16" s="7"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="9"/>
+      <c r="W16" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O17" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="T17" s="11"/>
+      <c r="U17" s="12"/>
+      <c r="W17" s="15"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O18" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O19" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O16" s="10" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O20" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="R22" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="S22" s="6"/>
+      <c r="U22" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" t="s">
+        <v>153</v>
+      </c>
+      <c r="R23" s="7">
+        <v>1</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="U23" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" t="s">
+        <v>154</v>
+      </c>
+      <c r="R24" s="7">
+        <v>2</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U24" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25" t="s">
+        <v>155</v>
+      </c>
+      <c r="R25" s="7">
+        <v>3</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" t="s">
+        <v>156</v>
+      </c>
+      <c r="R26" s="7">
+        <v>4</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="U26" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R18" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="S18" s="6"/>
-      <c r="U18" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R27" s="10">
+        <v>5</v>
+      </c>
+      <c r="S27" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="U27" s="14"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>32</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28" t="s">
+        <v>11</v>
+      </c>
+      <c r="O28" t="s">
+        <v>25</v>
+      </c>
+      <c r="U28" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="J29" t="s">
+        <v>31</v>
+      </c>
+      <c r="O29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
         <v>23</v>
       </c>
-      <c r="J19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" t="s">
-        <v>153</v>
-      </c>
-      <c r="R19" s="7">
+      <c r="U31" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="W31" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32">
         <v>1</v>
       </c>
-      <c r="S19" s="9" t="s">
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="U32" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="W32" s="14"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="U33" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="W33" s="14"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H34">
+        <v>3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
+      <c r="U34" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="W34" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>9</v>
+      </c>
+      <c r="U35" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>10</v>
+      </c>
+      <c r="U36" s="14"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="U37" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" t="s">
+        <v>141</v>
+      </c>
+      <c r="K41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I42" t="s">
+        <v>142</v>
+      </c>
+      <c r="K42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>143</v>
+      </c>
+      <c r="K43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
+        <v>144</v>
+      </c>
+      <c r="K44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" t="s">
+        <v>145</v>
+      </c>
+      <c r="K45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" t="s">
+        <v>146</v>
+      </c>
+      <c r="K46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="D47">
         <v>7</v>
       </c>
-      <c r="U19" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="I47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="I48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="I49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="D51">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" t="s">
-        <v>140</v>
-      </c>
-      <c r="H20">
+      <c r="E51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F58" t="s">
+        <v>50</v>
+      </c>
+      <c r="H58" t="s">
+        <v>61</v>
+      </c>
+      <c r="J58" t="s">
+        <v>68</v>
+      </c>
+      <c r="L58" t="s">
+        <v>78</v>
+      </c>
+      <c r="N58" t="s">
+        <v>86</v>
+      </c>
+      <c r="P58" t="s">
+        <v>93</v>
+      </c>
+      <c r="R58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="E59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59">
         <v>1</v>
       </c>
-      <c r="I20" t="s">
+      <c r="G59" t="s">
+        <v>52</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59" t="s">
+        <v>133</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59" t="s">
+        <v>69</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59" t="s">
+        <v>79</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59" t="s">
+        <v>87</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>94</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="E60" t="s">
+        <v>77</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60" t="s">
+        <v>56</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60" t="s">
+        <v>62</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60" t="s">
+        <v>71</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="M60" t="s">
+        <v>80</v>
+      </c>
+      <c r="N60">
+        <v>2</v>
+      </c>
+      <c r="O60" t="s">
+        <v>88</v>
+      </c>
+      <c r="P60">
+        <v>2</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>132</v>
+      </c>
+      <c r="R60">
+        <v>2</v>
+      </c>
+      <c r="S60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="E61" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61" t="s">
+        <v>57</v>
+      </c>
+      <c r="H61">
+        <v>3</v>
+      </c>
+      <c r="I61" t="s">
+        <v>63</v>
+      </c>
+      <c r="J61">
+        <v>3</v>
+      </c>
+      <c r="K61" t="s">
+        <v>70</v>
+      </c>
+      <c r="L61">
+        <v>3</v>
+      </c>
+      <c r="M61" t="s">
+        <v>81</v>
+      </c>
+      <c r="N61">
+        <v>3</v>
+      </c>
+      <c r="O61" t="s">
+        <v>89</v>
+      </c>
+      <c r="P61">
+        <v>3</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>95</v>
+      </c>
+      <c r="R61">
+        <v>3</v>
+      </c>
+      <c r="S61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F62">
+        <v>4</v>
+      </c>
+      <c r="G62" t="s">
+        <v>58</v>
+      </c>
+      <c r="H62">
+        <v>4</v>
+      </c>
+      <c r="I62" t="s">
+        <v>64</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+      <c r="K62" t="s">
+        <v>72</v>
+      </c>
+      <c r="L62">
+        <v>4</v>
+      </c>
+      <c r="M62" t="s">
+        <v>82</v>
+      </c>
+      <c r="N62">
+        <v>4</v>
+      </c>
+      <c r="O62" t="s">
+        <v>90</v>
+      </c>
+      <c r="P62">
+        <v>4</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>98</v>
+      </c>
+      <c r="R62">
+        <v>4</v>
+      </c>
+      <c r="S62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="G63" t="s">
+        <v>59</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63" t="s">
+        <v>65</v>
+      </c>
+      <c r="J63">
+        <v>5</v>
+      </c>
+      <c r="K63" t="s">
+        <v>73</v>
+      </c>
+      <c r="L63">
+        <v>5</v>
+      </c>
+      <c r="M63" t="s">
+        <v>83</v>
+      </c>
+      <c r="N63">
+        <v>5</v>
+      </c>
+      <c r="O63" t="s">
+        <v>91</v>
+      </c>
+      <c r="P63">
+        <v>5</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>97</v>
+      </c>
+      <c r="R63">
+        <v>5</v>
+      </c>
+      <c r="S63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F64">
+        <v>6</v>
+      </c>
+      <c r="G64" t="s">
+        <v>60</v>
+      </c>
+      <c r="H64">
+        <v>6</v>
+      </c>
+      <c r="I64" t="s">
+        <v>66</v>
+      </c>
+      <c r="J64">
+        <v>6</v>
+      </c>
+      <c r="K64" t="s">
+        <v>74</v>
+      </c>
+      <c r="L64">
+        <v>6</v>
+      </c>
+      <c r="M64" t="s">
+        <v>84</v>
+      </c>
+      <c r="N64">
+        <v>6</v>
+      </c>
+      <c r="O64" t="s">
+        <v>92</v>
+      </c>
+      <c r="P64">
+        <v>6</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>96</v>
+      </c>
+      <c r="R64">
+        <v>6</v>
+      </c>
+      <c r="S64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F65">
         <v>7</v>
       </c>
-      <c r="J20" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20">
+      <c r="G65" t="s">
+        <v>40</v>
+      </c>
+      <c r="H65">
+        <v>7</v>
+      </c>
+      <c r="I65" t="s">
+        <v>67</v>
+      </c>
+      <c r="J65">
+        <v>7</v>
+      </c>
+      <c r="K65" t="s">
+        <v>75</v>
+      </c>
+      <c r="L65">
+        <v>7</v>
+      </c>
+      <c r="M65" t="s">
+        <v>85</v>
+      </c>
+      <c r="N65">
+        <v>7</v>
+      </c>
+      <c r="O65" t="s">
+        <v>40</v>
+      </c>
+      <c r="P65">
+        <v>7</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H66">
+        <v>8</v>
+      </c>
+      <c r="I66" t="s">
+        <v>40</v>
+      </c>
+      <c r="J66">
+        <v>8</v>
+      </c>
+      <c r="K66" t="s">
+        <v>76</v>
+      </c>
+      <c r="L66">
+        <v>8</v>
+      </c>
+      <c r="M66" t="s">
+        <v>40</v>
+      </c>
+      <c r="P66">
+        <v>8</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="J67">
+        <v>9</v>
+      </c>
+      <c r="K67" t="s">
+        <v>40</v>
+      </c>
+      <c r="P67">
+        <v>9</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F69" t="s">
+        <v>51</v>
+      </c>
+      <c r="H69" t="s">
+        <v>61</v>
+      </c>
+      <c r="J69" t="s">
+        <v>108</v>
+      </c>
+      <c r="L69" t="s">
+        <v>109</v>
+      </c>
+      <c r="N69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F70">
         <v>1</v>
       </c>
-      <c r="M20" t="s">
-        <v>12</v>
-      </c>
-      <c r="O20" t="s">
-        <v>154</v>
-      </c>
-      <c r="R20" s="7">
+      <c r="G70" t="s">
+        <v>52</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70" t="s">
+        <v>123</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>118</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70" t="s">
+        <v>116</v>
+      </c>
+      <c r="N70">
+        <v>1</v>
+      </c>
+      <c r="O70" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F71">
         <v>2</v>
       </c>
-      <c r="S20" s="9" t="s">
+      <c r="G71" t="s">
+        <v>53</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71" t="s">
+        <v>124</v>
+      </c>
+      <c r="J71">
+        <v>2</v>
+      </c>
+      <c r="K71" t="s">
+        <v>119</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71" t="s">
+        <v>117</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
+      </c>
+      <c r="O71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F72">
+        <v>3</v>
+      </c>
+      <c r="G72" t="s">
+        <v>54</v>
+      </c>
+      <c r="H72">
+        <v>3</v>
+      </c>
+      <c r="I72" t="s">
+        <v>125</v>
+      </c>
+      <c r="J72">
+        <v>3</v>
+      </c>
+      <c r="K72" t="s">
+        <v>120</v>
+      </c>
+      <c r="L72">
+        <v>3</v>
+      </c>
+      <c r="M72" t="s">
+        <v>40</v>
+      </c>
+      <c r="N72">
+        <v>3</v>
+      </c>
+      <c r="O72" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F73">
+        <v>4</v>
+      </c>
+      <c r="G73" t="s">
+        <v>55</v>
+      </c>
+      <c r="H73">
+        <v>4</v>
+      </c>
+      <c r="I73" t="s">
+        <v>126</v>
+      </c>
+      <c r="J73">
+        <v>4</v>
+      </c>
+      <c r="K73" t="s">
+        <v>121</v>
+      </c>
+      <c r="N73">
+        <v>4</v>
+      </c>
+      <c r="O73" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74" t="s">
+        <v>40</v>
+      </c>
+      <c r="H74">
+        <v>5</v>
+      </c>
+      <c r="I74" t="s">
+        <v>127</v>
+      </c>
+      <c r="J74">
+        <v>5</v>
+      </c>
+      <c r="K74" t="s">
+        <v>122</v>
+      </c>
+      <c r="N74">
+        <v>5</v>
+      </c>
+      <c r="O74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H75">
+        <v>6</v>
+      </c>
+      <c r="I75" t="s">
+        <v>128</v>
+      </c>
+      <c r="J75">
+        <v>6</v>
+      </c>
+      <c r="K75" t="s">
+        <v>40</v>
+      </c>
+      <c r="N75">
+        <v>6</v>
+      </c>
+      <c r="O75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H76">
+        <v>7</v>
+      </c>
+      <c r="I76" t="s">
+        <v>129</v>
+      </c>
+      <c r="N76">
+        <v>7</v>
+      </c>
+      <c r="O76" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H77">
         <v>8</v>
       </c>
-      <c r="U20" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="I77" t="s">
+        <v>130</v>
+      </c>
+      <c r="N77">
         <v>8</v>
       </c>
-      <c r="J21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L21">
-        <v>2</v>
-      </c>
-      <c r="M21" t="s">
-        <v>13</v>
-      </c>
-      <c r="O21" t="s">
-        <v>155</v>
-      </c>
-      <c r="R21" s="7">
-        <v>3</v>
-      </c>
-      <c r="S21" s="9" t="s">
+      <c r="O77" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="H78">
         <v>9</v>
       </c>
-      <c r="U21" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L22">
-        <v>3</v>
-      </c>
-      <c r="M22" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" t="s">
-        <v>156</v>
-      </c>
-      <c r="R22" s="7">
-        <v>4</v>
-      </c>
-      <c r="S22" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="U22" s="14" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H23">
-        <v>4</v>
-      </c>
-      <c r="I23" t="s">
-        <v>10</v>
-      </c>
-      <c r="L23">
-        <v>4</v>
-      </c>
-      <c r="M23" t="s">
-        <v>15</v>
-      </c>
-      <c r="O23" t="s">
-        <v>24</v>
-      </c>
-      <c r="R23" s="10">
+      <c r="I78" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
         <v>5</v>
       </c>
-      <c r="S23" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="U23" s="14"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H24">
-        <v>5</v>
-      </c>
-      <c r="I24" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" t="s">
-        <v>32</v>
-      </c>
-      <c r="L24">
-        <v>5</v>
-      </c>
-      <c r="M24" t="s">
-        <v>11</v>
-      </c>
-      <c r="O24" t="s">
-        <v>25</v>
-      </c>
-      <c r="U24" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J25" t="s">
-        <v>31</v>
-      </c>
-      <c r="O25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" t="s">
-        <v>23</v>
-      </c>
-      <c r="U27" s="13"/>
-      <c r="W27" s="13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>19</v>
-      </c>
-      <c r="U28" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="W28" s="14"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29" t="s">
-        <v>20</v>
-      </c>
-      <c r="U29" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="W29" s="14"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H30">
-        <v>3</v>
-      </c>
-      <c r="I30" t="s">
-        <v>8</v>
-      </c>
-      <c r="U30" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="W30" s="15"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H31">
-        <v>4</v>
-      </c>
-      <c r="I31" t="s">
-        <v>9</v>
-      </c>
-      <c r="U31" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H32">
-        <v>5</v>
-      </c>
-      <c r="I32" t="s">
-        <v>10</v>
-      </c>
-      <c r="U32" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H33">
-        <v>6</v>
-      </c>
-      <c r="I33" t="s">
-        <v>11</v>
-      </c>
-      <c r="U33" s="14"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U34" s="14"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U35" s="14"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>3</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-      <c r="U36" s="15"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" t="s">
-        <v>141</v>
-      </c>
-      <c r="K37" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
-        <v>35</v>
-      </c>
-      <c r="I38" t="s">
-        <v>142</v>
-      </c>
-      <c r="K38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D39">
-        <v>3</v>
-      </c>
-      <c r="E39" t="s">
-        <v>36</v>
-      </c>
-      <c r="I39" t="s">
-        <v>143</v>
-      </c>
-      <c r="K39" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40" t="s">
-        <v>37</v>
-      </c>
-      <c r="I40" t="s">
-        <v>144</v>
-      </c>
-      <c r="K40" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D41">
-        <v>5</v>
-      </c>
-      <c r="E41" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" t="s">
-        <v>145</v>
-      </c>
-      <c r="K41" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D42">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>39</v>
-      </c>
-      <c r="I42" t="s">
-        <v>146</v>
-      </c>
-      <c r="K42" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D43">
-        <v>7</v>
-      </c>
-      <c r="E43" t="s">
-        <v>40</v>
-      </c>
-      <c r="I43" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I44" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>4</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D49">
-        <v>3</v>
-      </c>
-      <c r="E49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D50">
-        <v>4</v>
-      </c>
-      <c r="E50" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>5</v>
-      </c>
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" t="s">
-        <v>48</v>
-      </c>
-      <c r="F54" t="s">
-        <v>50</v>
-      </c>
-      <c r="H54" t="s">
-        <v>61</v>
-      </c>
-      <c r="J54" t="s">
-        <v>68</v>
-      </c>
-      <c r="L54" t="s">
-        <v>78</v>
-      </c>
-      <c r="N54" t="s">
-        <v>86</v>
-      </c>
-      <c r="P54" t="s">
-        <v>93</v>
-      </c>
-      <c r="R54" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55" t="s">
-        <v>52</v>
-      </c>
-      <c r="H55">
-        <v>1</v>
-      </c>
-      <c r="I55" t="s">
-        <v>133</v>
-      </c>
-      <c r="J55">
-        <v>1</v>
-      </c>
-      <c r="K55" t="s">
-        <v>69</v>
-      </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-      <c r="M55" t="s">
-        <v>79</v>
-      </c>
-      <c r="N55">
-        <v>1</v>
-      </c>
-      <c r="O55" t="s">
-        <v>87</v>
-      </c>
-      <c r="P55">
-        <v>1</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>94</v>
-      </c>
-      <c r="R55">
-        <v>1</v>
-      </c>
-      <c r="S55" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
-        <v>77</v>
-      </c>
-      <c r="F56">
-        <v>2</v>
-      </c>
-      <c r="G56" t="s">
-        <v>56</v>
-      </c>
-      <c r="H56">
-        <v>2</v>
-      </c>
-      <c r="I56" t="s">
-        <v>62</v>
-      </c>
-      <c r="J56">
-        <v>2</v>
-      </c>
-      <c r="K56" t="s">
-        <v>71</v>
-      </c>
-      <c r="L56">
-        <v>2</v>
-      </c>
-      <c r="M56" t="s">
-        <v>80</v>
-      </c>
-      <c r="N56">
-        <v>2</v>
-      </c>
-      <c r="O56" t="s">
-        <v>88</v>
-      </c>
-      <c r="P56">
-        <v>2</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>132</v>
-      </c>
-      <c r="R56">
-        <v>2</v>
-      </c>
-      <c r="S56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E57" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57">
-        <v>3</v>
-      </c>
-      <c r="G57" t="s">
-        <v>57</v>
-      </c>
-      <c r="H57">
-        <v>3</v>
-      </c>
-      <c r="I57" t="s">
-        <v>63</v>
-      </c>
-      <c r="J57">
-        <v>3</v>
-      </c>
-      <c r="K57" t="s">
-        <v>70</v>
-      </c>
-      <c r="L57">
-        <v>3</v>
-      </c>
-      <c r="M57" t="s">
-        <v>81</v>
-      </c>
-      <c r="N57">
-        <v>3</v>
-      </c>
-      <c r="O57" t="s">
-        <v>89</v>
-      </c>
-      <c r="P57">
-        <v>3</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>95</v>
-      </c>
-      <c r="R57">
-        <v>3</v>
-      </c>
-      <c r="S57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F58">
-        <v>4</v>
-      </c>
-      <c r="G58" t="s">
-        <v>58</v>
-      </c>
-      <c r="H58">
-        <v>4</v>
-      </c>
-      <c r="I58" t="s">
-        <v>64</v>
-      </c>
-      <c r="J58">
-        <v>4</v>
-      </c>
-      <c r="K58" t="s">
-        <v>72</v>
-      </c>
-      <c r="L58">
-        <v>4</v>
-      </c>
-      <c r="M58" t="s">
-        <v>82</v>
-      </c>
-      <c r="N58">
-        <v>4</v>
-      </c>
-      <c r="O58" t="s">
-        <v>90</v>
-      </c>
-      <c r="P58">
-        <v>4</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>98</v>
-      </c>
-      <c r="R58">
-        <v>4</v>
-      </c>
-      <c r="S58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F59">
-        <v>5</v>
-      </c>
-      <c r="G59" t="s">
-        <v>59</v>
-      </c>
-      <c r="H59">
-        <v>5</v>
-      </c>
-      <c r="I59" t="s">
-        <v>65</v>
-      </c>
-      <c r="J59">
-        <v>5</v>
-      </c>
-      <c r="K59" t="s">
-        <v>73</v>
-      </c>
-      <c r="L59">
-        <v>5</v>
-      </c>
-      <c r="M59" t="s">
-        <v>83</v>
-      </c>
-      <c r="N59">
-        <v>5</v>
-      </c>
-      <c r="O59" t="s">
-        <v>91</v>
-      </c>
-      <c r="P59">
-        <v>5</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>97</v>
-      </c>
-      <c r="R59">
-        <v>5</v>
-      </c>
-      <c r="S59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F60">
-        <v>6</v>
-      </c>
-      <c r="G60" t="s">
-        <v>60</v>
-      </c>
-      <c r="H60">
-        <v>6</v>
-      </c>
-      <c r="I60" t="s">
-        <v>66</v>
-      </c>
-      <c r="J60">
-        <v>6</v>
-      </c>
-      <c r="K60" t="s">
-        <v>74</v>
-      </c>
-      <c r="L60">
-        <v>6</v>
-      </c>
-      <c r="M60" t="s">
-        <v>84</v>
-      </c>
-      <c r="N60">
-        <v>6</v>
-      </c>
-      <c r="O60" t="s">
-        <v>92</v>
-      </c>
-      <c r="P60">
-        <v>6</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>96</v>
-      </c>
-      <c r="R60">
-        <v>6</v>
-      </c>
-      <c r="S60" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F61">
-        <v>7</v>
-      </c>
-      <c r="G61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H61">
-        <v>7</v>
-      </c>
-      <c r="I61" t="s">
-        <v>67</v>
-      </c>
-      <c r="J61">
-        <v>7</v>
-      </c>
-      <c r="K61" t="s">
-        <v>75</v>
-      </c>
-      <c r="L61">
-        <v>7</v>
-      </c>
-      <c r="M61" t="s">
-        <v>85</v>
-      </c>
-      <c r="N61">
-        <v>7</v>
-      </c>
-      <c r="O61" t="s">
-        <v>40</v>
-      </c>
-      <c r="P61">
-        <v>7</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H62">
-        <v>8</v>
-      </c>
-      <c r="I62" t="s">
-        <v>40</v>
-      </c>
-      <c r="J62">
-        <v>8</v>
-      </c>
-      <c r="K62" t="s">
-        <v>76</v>
-      </c>
-      <c r="L62">
-        <v>8</v>
-      </c>
-      <c r="M62" t="s">
-        <v>40</v>
-      </c>
-      <c r="P62">
-        <v>8</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J63">
-        <v>9</v>
-      </c>
-      <c r="K63" t="s">
-        <v>40</v>
-      </c>
-      <c r="P63">
-        <v>9</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F65" t="s">
-        <v>51</v>
-      </c>
-      <c r="H65" t="s">
-        <v>61</v>
-      </c>
-      <c r="J65" t="s">
-        <v>108</v>
-      </c>
-      <c r="L65" t="s">
-        <v>109</v>
-      </c>
-      <c r="N65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66" t="s">
-        <v>52</v>
-      </c>
-      <c r="H66">
-        <v>1</v>
-      </c>
-      <c r="I66" t="s">
-        <v>123</v>
-      </c>
-      <c r="J66">
-        <v>1</v>
-      </c>
-      <c r="K66" t="s">
-        <v>118</v>
-      </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-      <c r="M66" t="s">
-        <v>116</v>
-      </c>
-      <c r="N66">
-        <v>1</v>
-      </c>
-      <c r="O66" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F67">
-        <v>2</v>
-      </c>
-      <c r="G67" t="s">
-        <v>53</v>
-      </c>
-      <c r="H67">
-        <v>2</v>
-      </c>
-      <c r="I67" t="s">
-        <v>124</v>
-      </c>
-      <c r="J67">
-        <v>2</v>
-      </c>
-      <c r="K67" t="s">
-        <v>119</v>
-      </c>
-      <c r="L67">
-        <v>2</v>
-      </c>
-      <c r="M67" t="s">
-        <v>117</v>
-      </c>
-      <c r="N67">
-        <v>2</v>
-      </c>
-      <c r="O67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F68">
-        <v>3</v>
-      </c>
-      <c r="G68" t="s">
-        <v>54</v>
-      </c>
-      <c r="H68">
-        <v>3</v>
-      </c>
-      <c r="I68" t="s">
-        <v>125</v>
-      </c>
-      <c r="J68">
-        <v>3</v>
-      </c>
-      <c r="K68" t="s">
-        <v>120</v>
-      </c>
-      <c r="L68">
-        <v>3</v>
-      </c>
-      <c r="M68" t="s">
-        <v>40</v>
-      </c>
-      <c r="N68">
-        <v>3</v>
-      </c>
-      <c r="O68" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F69">
-        <v>4</v>
-      </c>
-      <c r="G69" t="s">
-        <v>55</v>
-      </c>
-      <c r="H69">
-        <v>4</v>
-      </c>
-      <c r="I69" t="s">
-        <v>126</v>
-      </c>
-      <c r="J69">
-        <v>4</v>
-      </c>
-      <c r="K69" t="s">
-        <v>121</v>
-      </c>
-      <c r="N69">
-        <v>4</v>
-      </c>
-      <c r="O69" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F70">
-        <v>5</v>
-      </c>
-      <c r="G70" t="s">
-        <v>40</v>
-      </c>
-      <c r="H70">
-        <v>5</v>
-      </c>
-      <c r="I70" t="s">
-        <v>127</v>
-      </c>
-      <c r="J70">
-        <v>5</v>
-      </c>
-      <c r="K70" t="s">
-        <v>122</v>
-      </c>
-      <c r="N70">
-        <v>5</v>
-      </c>
-      <c r="O70" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H71">
-        <v>6</v>
-      </c>
-      <c r="I71" t="s">
-        <v>128</v>
-      </c>
-      <c r="J71">
-        <v>6</v>
-      </c>
-      <c r="K71" t="s">
-        <v>40</v>
-      </c>
-      <c r="N71">
-        <v>6</v>
-      </c>
-      <c r="O71" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H72">
-        <v>7</v>
-      </c>
-      <c r="I72" t="s">
-        <v>129</v>
-      </c>
-      <c r="N72">
-        <v>7</v>
-      </c>
-      <c r="O72" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H73">
-        <v>8</v>
-      </c>
-      <c r="I73" t="s">
-        <v>130</v>
-      </c>
-      <c r="N73">
-        <v>8</v>
-      </c>
-      <c r="O73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H74">
-        <v>9</v>
-      </c>
-      <c r="I74" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>6</v>
-      </c>
-      <c r="B76" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="E80" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E81" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E82" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4667,20 +4826,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.15">
       <c r="C5" s="1" t="s">
         <v>160</v>
       </c>
@@ -4709,7 +4868,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.15">
       <c r="E8" s="3">
         <v>1</v>
       </c>
@@ -4723,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.15">
       <c r="E9" s="2">
         <v>2</v>
       </c>
@@ -4737,7 +4896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F10">
         <v>3</v>
       </c>
@@ -4748,7 +4907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F11">
         <v>4</v>
       </c>
@@ -4759,7 +4918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F12">
         <v>5</v>
       </c>
@@ -4770,7 +4929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.15">
       <c r="F13">
         <v>6</v>
       </c>
@@ -4781,7 +4940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.15">
       <c r="G14">
         <v>7</v>
       </c>
@@ -4789,7 +4948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.15">
       <c r="G15">
         <v>8</v>
       </c>
@@ -4797,7 +4956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.15">
       <c r="G16">
         <v>9</v>
       </c>
@@ -4805,7 +4964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G17">
         <v>10</v>
       </c>
@@ -4813,7 +4972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G18">
         <v>11</v>
       </c>
@@ -4821,7 +4980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G19">
         <v>12</v>
       </c>
@@ -4829,57 +4988,57 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H20" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H21" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H22" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H23" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H24" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H25" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H26" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H27" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H28" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H29" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:8" x14ac:dyDescent="0.15">
       <c r="H30" s="3">
         <v>23</v>
       </c>
@@ -4891,12 +5050,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add 8009 doc and DataParse.cs temp file
</commit_message>
<xml_diff>
--- a/doc/水表功能列表.xlsx
+++ b/doc/水表功能列表.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="212">
   <si>
     <t>表端</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -650,38 +648,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>No.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>楼栋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>集中器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>户号/表号/门牌号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>返回   &lt;完成&gt;  继续</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -890,6 +856,10 @@
   </si>
   <si>
     <t>返回         户表命令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空抄表结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -913,24 +883,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1074,11 +1032,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1092,8 +1047,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1131,7 +1086,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1184,7 +1139,7 @@
         <xdr:cNvPr id="5" name="直接箭头连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1237,7 +1192,7 @@
         <xdr:cNvPr id="7" name="直接箭头连接符 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,7 +1245,7 @@
         <xdr:cNvPr id="12" name="直接箭头连接符 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1298,7 @@
         <xdr:cNvPr id="14" name="直接箭头连接符 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1396,7 +1351,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1449,7 +1404,7 @@
         <xdr:cNvPr id="25" name="直接箭头连接符 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1502,7 +1457,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1555,7 +1510,7 @@
         <xdr:cNvPr id="32" name="直接箭头连接符 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1608,7 +1563,7 @@
         <xdr:cNvPr id="34" name="直接箭头连接符 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1661,7 +1616,7 @@
         <xdr:cNvPr id="38" name="直接箭头连接符 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1714,7 +1669,7 @@
         <xdr:cNvPr id="39" name="直接箭头连接符 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1767,7 +1722,7 @@
         <xdr:cNvPr id="58" name="直接箭头连接符 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1820,7 +1775,7 @@
         <xdr:cNvPr id="59" name="直接箭头连接符 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1873,7 +1828,7 @@
         <xdr:cNvPr id="60" name="直接箭头连接符 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1881,7 @@
         <xdr:cNvPr id="66" name="直接箭头连接符 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1979,7 +1934,7 @@
         <xdr:cNvPr id="20" name="直接箭头连接符 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2032,7 +1987,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2085,7 +2040,7 @@
         <xdr:cNvPr id="26" name="直接箭头连接符 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2138,7 +2093,7 @@
         <xdr:cNvPr id="54" name="直接箭头连接符 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2191,7 +2146,7 @@
         <xdr:cNvPr id="55" name="直接箭头连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2244,7 +2199,7 @@
         <xdr:cNvPr id="57" name="直接箭头连接符 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2297,7 +2252,7 @@
         <xdr:cNvPr id="64" name="直接箭头连接符 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2350,7 +2305,7 @@
         <xdr:cNvPr id="65" name="直接箭头连接符 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2403,7 +2358,7 @@
         <xdr:cNvPr id="67" name="直接箭头连接符 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2456,7 +2411,7 @@
         <xdr:cNvPr id="68" name="直接箭头连接符 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2509,7 +2464,7 @@
         <xdr:cNvPr id="70" name="直接箭头连接符 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2562,7 +2517,7 @@
         <xdr:cNvPr id="71" name="直接箭头连接符 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2615,7 +2570,7 @@
         <xdr:cNvPr id="72" name="直接箭头连接符 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2668,7 +2623,7 @@
         <xdr:cNvPr id="73" name="直接箭头连接符 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2721,7 +2676,7 @@
         <xdr:cNvPr id="74" name="直接箭头连接符 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2774,7 +2729,7 @@
         <xdr:cNvPr id="75" name="直接箭头连接符 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2827,7 +2782,7 @@
         <xdr:cNvPr id="76" name="直接箭头连接符 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2880,7 +2835,7 @@
         <xdr:cNvPr id="77" name="直接箭头连接符 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2933,7 +2888,7 @@
         <xdr:cNvPr id="78" name="直接箭头连接符 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2986,7 +2941,7 @@
         <xdr:cNvPr id="79" name="直接箭头连接符 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3039,7 +2994,7 @@
         <xdr:cNvPr id="80" name="直接箭头连接符 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3366,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3398,25 +3353,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4">
@@ -4461,60 +4416,60 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
-      <c r="Q75" s="17"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+      <c r="Q75" s="14"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I78" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="K78" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="M78" s="13"/>
-      <c r="O78" s="13"/>
+      <c r="I78" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="K78" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="M78" s="10"/>
+      <c r="O78" s="10"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.15">
       <c r="E79" t="s">
-        <v>214</v>
-      </c>
-      <c r="I79" s="14"/>
-      <c r="K79" s="14"/>
-      <c r="M79" s="14"/>
-      <c r="O79" s="14"/>
+        <v>206</v>
+      </c>
+      <c r="I79" s="11"/>
+      <c r="K79" s="11"/>
+      <c r="M79" s="11"/>
+      <c r="O79" s="11"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I80" s="14"/>
-      <c r="K80" s="14"/>
-      <c r="M80" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="O80" s="14" t="s">
-        <v>196</v>
+      <c r="I80" s="11"/>
+      <c r="K80" s="11"/>
+      <c r="M80" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="O80" s="11" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I81" s="14"/>
-      <c r="K81" s="14"/>
-      <c r="M81" s="14"/>
-      <c r="O81" s="14"/>
+      <c r="I81" s="11"/>
+      <c r="K81" s="11"/>
+      <c r="M81" s="11"/>
+      <c r="O81" s="11"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A82">
@@ -4527,16 +4482,16 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>177</v>
-      </c>
-      <c r="I82" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="K82" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="M82" s="15"/>
-      <c r="O82" s="15"/>
+        <v>169</v>
+      </c>
+      <c r="I82" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="K82" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="M82" s="12"/>
+      <c r="O82" s="12"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A83">
@@ -4549,7 +4504,7 @@
         <v>2</v>
       </c>
       <c r="G83" t="s">
-        <v>43</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.15">
@@ -4565,17 +4520,17 @@
       <c r="G84" t="s">
         <v>137</v>
       </c>
-      <c r="I84" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="M84" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="N84" s="5"/>
-      <c r="O84" s="6"/>
+      <c r="I84" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N84" s="2"/>
+      <c r="O84" s="3"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A85">
@@ -4588,20 +4543,20 @@
         <v>4</v>
       </c>
       <c r="G85" t="s">
-        <v>179</v>
-      </c>
-      <c r="I85" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="K85" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="M85" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="K85" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="M85" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N85" s="8"/>
-      <c r="O85" s="9" t="s">
-        <v>174</v>
+      <c r="N85" s="5"/>
+      <c r="O85" s="6" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.15">
@@ -4617,16 +4572,16 @@
       <c r="G86" t="s">
         <v>10</v>
       </c>
-      <c r="I86" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="K86" s="14"/>
-      <c r="M86" s="7" t="s">
+      <c r="I86" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="K86" s="11"/>
+      <c r="M86" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N86" s="8"/>
-      <c r="O86" s="9" t="s">
-        <v>171</v>
+      <c r="N86" s="5"/>
+      <c r="O86" s="6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.15">
@@ -4636,16 +4591,16 @@
       <c r="B87" t="s">
         <v>65</v>
       </c>
-      <c r="I87" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="K87" s="14"/>
-      <c r="M87" s="7" t="s">
+      <c r="I87" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="K87" s="11"/>
+      <c r="M87" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="N87" s="8"/>
-      <c r="O87" s="9" t="s">
-        <v>172</v>
+      <c r="N87" s="5"/>
+      <c r="O87" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.15">
@@ -4655,21 +4610,21 @@
       <c r="B88" t="s">
         <v>4</v>
       </c>
-      <c r="I88" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="K88" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="M88" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="N88" s="8"/>
-      <c r="O88" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q88" s="13" t="s">
-        <v>192</v>
+      <c r="I88" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="K88" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="N88" s="5"/>
+      <c r="O88" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q88" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.15">
@@ -4679,196 +4634,196 @@
       <c r="B89" t="s">
         <v>134</v>
       </c>
-      <c r="M89" s="16" t="s">
+      <c r="M89" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="N89" s="8"/>
-      <c r="O89" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q89" s="14" t="s">
+      <c r="N89" s="5"/>
+      <c r="O89" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q89" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I90" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="K90" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="N90" s="5"/>
+      <c r="O90" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q90" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I91" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="K91" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="M91" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N91" s="5"/>
+      <c r="O91" s="6"/>
+      <c r="Q91" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I92" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="K92" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="M92" s="4"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="6"/>
+      <c r="Q92" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I93" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="K93" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M93" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="N93" s="8"/>
+      <c r="O93" s="9"/>
+      <c r="Q93" s="12"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I94" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K94" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I95" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="K95" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="I96" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="K96" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M98" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="O98" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M99" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="O99" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M100" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="O100" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M101" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="O101" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M102" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="O102" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M103" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="O103" s="11"/>
+    </row>
+    <row r="104" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="M104" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="O104" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="107" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="O107" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I90" s="13" t="s">
+      <c r="Q107" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="108" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="O108" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q108" s="11"/>
+    </row>
+    <row r="109" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="O109" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="K90" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="M90" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="N90" s="8"/>
-      <c r="O90" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q90" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I91" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="K91" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="M91" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N91" s="8"/>
-      <c r="O91" s="9"/>
-      <c r="Q91" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I92" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="K92" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="M92" s="7"/>
-      <c r="N92" s="8"/>
-      <c r="O92" s="9"/>
-      <c r="Q92" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I93" s="14" t="s">
+      <c r="Q109" s="11"/>
+    </row>
+    <row r="110" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="O110" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q110" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="K93" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M93" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="N93" s="11"/>
-      <c r="O93" s="12"/>
-      <c r="Q93" s="15"/>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I94" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="K94" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I95" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="K95" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I96" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="K96" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="98" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M98" s="13" t="s">
+    </row>
+    <row r="111" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="O111" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="13:17" x14ac:dyDescent="0.15">
+      <c r="O112" s="11"/>
+    </row>
+    <row r="113" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O113" s="12" t="s">
         <v>198</v>
-      </c>
-      <c r="O98" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="99" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M99" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="O99" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="100" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M100" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="O100" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="101" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M101" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="O101" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="102" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M102" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="O102" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="103" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M103" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="O103" s="14"/>
-    </row>
-    <row r="104" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M104" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="O104" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="107" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O107" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q107" s="13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="108" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O108" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q108" s="14"/>
-    </row>
-    <row r="109" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O109" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q109" s="14"/>
-    </row>
-    <row r="110" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O110" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q110" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="111" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O111" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="112" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O112" s="14"/>
-    </row>
-    <row r="113" spans="15:15" x14ac:dyDescent="0.15">
-      <c r="O113" s="15" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4877,241 +4832,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:M30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="13" max="13" width="17.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="C5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K5" t="s">
-        <v>163</v>
-      </c>
-      <c r="L5" t="s">
-        <v>164</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="F13">
-        <v>6</v>
-      </c>
-      <c r="G13">
-        <v>6</v>
-      </c>
-      <c r="H13" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="G14">
-        <v>7</v>
-      </c>
-      <c r="H14" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="G15">
-        <v>8</v>
-      </c>
-      <c r="H15" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.15">
-      <c r="G16">
-        <v>9</v>
-      </c>
-      <c r="H16" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="G18">
-        <v>11</v>
-      </c>
-      <c r="H18" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="G19">
-        <v>12</v>
-      </c>
-      <c r="H19" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H20" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H21" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H22" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H23" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H24" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H25" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H26" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H27" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H28" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H29" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.15">
-      <c r="H30" s="3">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add upgrade ui design doc
</commit_message>
<xml_diff>
--- a/doc/水表功能列表.xlsx
+++ b/doc/水表功能列表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="249">
   <si>
     <t>表端</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -739,10 +739,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;&lt;已抄/未抄列表    n/m</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -827,11 +823,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>小区选择：全部/单个</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>楼栋选择：全部/单个</t>
+    <t>清空中… -&gt; 已清空！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新版本（A380）手持机功能列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老版本（HT2900）手持机功能列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回         户表命令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空抄表结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.小区选择：全部/单个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.楼栋选择：全部/单个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.统计</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -839,27 +859,156 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>返回           确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;抄表统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;批量抄表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;程序升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.选择升级文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.查询升级状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.输入表号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  &gt; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;开始升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表号：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">返回    &lt;升级中&gt;     </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前-&gt; 发送升级数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本：v1.2  CRC：ADFE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本：v1.2  CRC：ADFE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前版本：v1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级状态：缺包等待</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.开始升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级状态：升级完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前版本：v1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前缺包：1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前缺包：20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前发包：190 / 200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>限制条件：无,可以升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>限制条件：无,可以升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;查询升级状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前-&gt;通知开始升级a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前-&gt;通知开始升级b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前-&gt; 查询升级状态b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前-&gt; 查询升级状态a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前-&gt; 查询升级状态b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;查询升级状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">返回  &lt;查询中/完成&gt; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">返回  &lt;查询中/完成&gt;   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">v1.2-ADFE 未开始/
+已完成/缺包等待  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.2-ADFE 文件OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>对应老版本的"工程调试"-&gt;"表端操作"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>清空中… -&gt; 已清空！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新版本（A380）手持机功能列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>老版本（HT2900）手持机功能列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回         户表命令</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>清空抄表结果</t>
+    <t>"工程调试"-&gt;"程序升级"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -903,7 +1052,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1028,11 +1177,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1049,6 +1213,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1086,7 +1253,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1139,7 +1306,7 @@
         <xdr:cNvPr id="5" name="直接箭头连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1192,7 +1359,7 @@
         <xdr:cNvPr id="7" name="直接箭头连接符 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1245,7 +1412,7 @@
         <xdr:cNvPr id="12" name="直接箭头连接符 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1298,7 +1465,7 @@
         <xdr:cNvPr id="14" name="直接箭头连接符 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1351,7 +1518,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1404,7 +1571,7 @@
         <xdr:cNvPr id="25" name="直接箭头连接符 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1457,7 +1624,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1510,7 +1677,7 @@
         <xdr:cNvPr id="32" name="直接箭头连接符 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1563,7 +1730,7 @@
         <xdr:cNvPr id="34" name="直接箭头连接符 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1616,7 +1783,7 @@
         <xdr:cNvPr id="38" name="直接箭头连接符 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1669,7 +1836,7 @@
         <xdr:cNvPr id="39" name="直接箭头连接符 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1722,7 +1889,7 @@
         <xdr:cNvPr id="58" name="直接箭头连接符 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1775,7 +1942,7 @@
         <xdr:cNvPr id="59" name="直接箭头连接符 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1828,7 +1995,7 @@
         <xdr:cNvPr id="60" name="直接箭头连接符 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1881,7 +2048,7 @@
         <xdr:cNvPr id="66" name="直接箭头连接符 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1934,7 +2101,7 @@
         <xdr:cNvPr id="20" name="直接箭头连接符 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1987,7 +2154,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2040,7 +2207,7 @@
         <xdr:cNvPr id="26" name="直接箭头连接符 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2093,7 +2260,7 @@
         <xdr:cNvPr id="54" name="直接箭头连接符 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2146,7 +2313,7 @@
         <xdr:cNvPr id="55" name="直接箭头连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2199,7 +2366,7 @@
         <xdr:cNvPr id="57" name="直接箭头连接符 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2252,7 +2419,7 @@
         <xdr:cNvPr id="64" name="直接箭头连接符 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2305,7 +2472,7 @@
         <xdr:cNvPr id="65" name="直接箭头连接符 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2358,7 +2525,7 @@
         <xdr:cNvPr id="67" name="直接箭头连接符 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2411,7 +2578,7 @@
         <xdr:cNvPr id="68" name="直接箭头连接符 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2464,7 +2631,7 @@
         <xdr:cNvPr id="70" name="直接箭头连接符 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2517,7 +2684,7 @@
         <xdr:cNvPr id="71" name="直接箭头连接符 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2570,7 +2737,7 @@
         <xdr:cNvPr id="72" name="直接箭头连接符 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2623,7 +2790,7 @@
         <xdr:cNvPr id="73" name="直接箭头连接符 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2676,7 +2843,7 @@
         <xdr:cNvPr id="74" name="直接箭头连接符 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2729,7 +2896,7 @@
         <xdr:cNvPr id="75" name="直接箭头连接符 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2782,7 +2949,7 @@
         <xdr:cNvPr id="76" name="直接箭头连接符 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2835,7 +3002,7 @@
         <xdr:cNvPr id="77" name="直接箭头连接符 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2888,7 +3055,7 @@
         <xdr:cNvPr id="78" name="直接箭头连接符 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2941,7 +3108,7 @@
         <xdr:cNvPr id="79" name="直接箭头连接符 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2994,7 +3161,7 @@
         <xdr:cNvPr id="80" name="直接箭头连接符 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3021,6 +3188,735 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>795618</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>268942</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>33619</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="直接箭头连接符 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3753971" y="20215412"/>
+          <a:ext cx="481853" cy="829236"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>795618</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直接箭头连接符 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3753971" y="21268765"/>
+          <a:ext cx="537882" cy="414617"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1355913</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>89648</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="直接箭头连接符 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5625354" y="22098000"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1411941</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>145676</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="直接箭头连接符 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5681382" y="20092147"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1344705</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>100852</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="直接箭头连接符 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7451911" y="20103353"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1535204</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>179292</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="直接箭头连接符 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11228292" y="20069735"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>773206</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="直接箭头连接符 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10533529" y="21067059"/>
+          <a:ext cx="11206" cy="403412"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>78442</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="直接箭头连接符 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11217088" y="20417118"/>
+          <a:ext cx="560294" cy="22411"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>201708</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>67237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>134472</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="直接箭头连接符 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6308914" y="22927237"/>
+          <a:ext cx="11204" cy="403411"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>78442</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="直接箭头连接符 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7732059" y="22983265"/>
+          <a:ext cx="2117912" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>336178</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>123267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="直接箭头连接符 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3294531" y="21638561"/>
+          <a:ext cx="2812675" cy="1781734"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="直接箭头连接符 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2846294" y="19543059"/>
+          <a:ext cx="0" cy="694765"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>941295</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1075765</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="肘形连接符 92"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5289177" y="19352559"/>
+          <a:ext cx="5558117" cy="257735"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>963706</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>963706</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="110" name="直接连接符 109"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5311588" y="19352559"/>
+          <a:ext cx="0" cy="224117"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -3319,10 +4215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S113"/>
+  <dimension ref="A2:S140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S131" sqref="S131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3333,11 +4229,11 @@
     <col min="4" max="4" width="4.125" customWidth="1"/>
     <col min="5" max="5" width="13.75" customWidth="1"/>
     <col min="6" max="6" width="4.25" customWidth="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="7" max="7" width="14.25" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
-    <col min="9" max="9" width="17.875" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="4.125" customWidth="1"/>
-    <col min="11" max="11" width="18.25" customWidth="1"/>
+    <col min="11" max="11" width="20.125" customWidth="1"/>
     <col min="12" max="12" width="3.625" customWidth="1"/>
     <col min="13" max="13" width="19.375" customWidth="1"/>
     <col min="14" max="14" width="3.75" customWidth="1"/>
@@ -3355,7 +4251,7 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -4418,7 +5314,7 @@
     <row r="75" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A75" s="14"/>
       <c r="B75" s="14" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
@@ -4438,20 +5334,20 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.15">
       <c r="I78" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="K78" s="10" t="s">
         <v>186</v>
-      </c>
-      <c r="K78" s="10" t="s">
-        <v>187</v>
       </c>
       <c r="M78" s="10"/>
       <c r="O78" s="10"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.15">
       <c r="E79" t="s">
-        <v>206</v>
-      </c>
-      <c r="I79" s="11"/>
-      <c r="K79" s="11"/>
+        <v>247</v>
+      </c>
+      <c r="I79" s="10"/>
+      <c r="K79" s="10"/>
       <c r="M79" s="11"/>
       <c r="O79" s="11"/>
     </row>
@@ -4459,15 +5355,19 @@
       <c r="I80" s="11"/>
       <c r="K80" s="11"/>
       <c r="M80" s="11" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="O80" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I81" s="11"/>
-      <c r="K81" s="11"/>
+      <c r="F81" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G81" s="3"/>
+      <c r="I81" s="12"/>
+      <c r="K81" s="12"/>
       <c r="M81" s="11"/>
       <c r="O81" s="11"/>
     </row>
@@ -4478,17 +5378,17 @@
       <c r="B82" t="s">
         <v>133</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="1">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="3" t="s">
         <v>169</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M82" s="12"/>
       <c r="O82" s="12"/>
@@ -4500,11 +5400,11 @@
       <c r="B83" t="s">
         <v>62</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="4">
         <v>2</v>
       </c>
-      <c r="G83" t="s">
-        <v>211</v>
+      <c r="G83" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.15">
@@ -4514,10 +5414,10 @@
       <c r="B84" t="s">
         <v>135</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="4">
         <v>3</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="6" t="s">
         <v>137</v>
       </c>
       <c r="I84" s="10" t="s">
@@ -4539,23 +5439,23 @@
       <c r="B85" t="s">
         <v>136</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="4">
         <v>4</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="I85" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="K85" s="11" t="s">
+      <c r="I85" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="K85" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="M85" s="4" t="s">
+      <c r="M85" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N85" s="5"/>
-      <c r="O85" s="6" t="s">
+      <c r="N85" s="2"/>
+      <c r="O85" s="3" t="s">
         <v>166</v>
       </c>
     </row>
@@ -4566,14 +5466,14 @@
       <c r="B86" t="s">
         <v>63</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="4">
         <v>5</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K86" s="11"/>
       <c r="M86" s="4" t="s">
@@ -4591,10 +5491,12 @@
       <c r="B87" t="s">
         <v>65</v>
       </c>
-      <c r="I87" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K87" s="11"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="6"/>
+      <c r="I87" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="K87" s="12"/>
       <c r="M87" s="4" t="s">
         <v>145</v>
       </c>
@@ -4610,8 +5512,10 @@
       <c r="B88" t="s">
         <v>4</v>
       </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="9"/>
       <c r="I88" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K88" s="12" t="s">
         <v>160</v>
@@ -4621,10 +5525,10 @@
       </c>
       <c r="N88" s="5"/>
       <c r="O88" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q88" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.15">
@@ -4634,6 +5538,10 @@
       <c r="B89" t="s">
         <v>134</v>
       </c>
+      <c r="F89" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G89" s="9"/>
       <c r="M89" s="13" t="s">
         <v>29</v>
       </c>
@@ -4641,13 +5549,13 @@
       <c r="O89" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="Q89" s="11" t="s">
+      <c r="Q89" s="10" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.15">
       <c r="I90" s="10" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="K90" s="10" t="s">
         <v>170</v>
@@ -4664,10 +5572,10 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I91" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="K91" s="11" t="s">
+      <c r="I91" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="K91" s="10" t="s">
         <v>154</v>
       </c>
       <c r="M91" s="4" t="s">
@@ -4681,27 +5589,27 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.15">
       <c r="I92" s="11" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="K92" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="M92" s="4"/>
-      <c r="N92" s="5"/>
-      <c r="O92" s="6"/>
+      <c r="M92" s="7"/>
+      <c r="N92" s="8"/>
+      <c r="O92" s="9"/>
       <c r="Q92" s="11" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.15">
       <c r="I93" s="11" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="K93" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M93" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="N93" s="8"/>
       <c r="O93" s="9"/>
@@ -4716,16 +5624,16 @@
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="I95" s="11" t="s">
+      <c r="I95" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="K95" s="11" t="s">
+      <c r="K95" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.15">
       <c r="I96" s="12" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="K96" s="12" t="s">
         <v>158</v>
@@ -4733,23 +5641,23 @@
     </row>
     <row r="98" spans="13:17" x14ac:dyDescent="0.15">
       <c r="M98" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O98" s="10" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="99" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="M99" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="O99" s="11" t="s">
+      <c r="M99" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="O99" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="100" spans="13:17" x14ac:dyDescent="0.15">
       <c r="M100" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O100" s="11" t="s">
         <v>29</v>
@@ -4757,7 +5665,7 @@
     </row>
     <row r="101" spans="13:17" x14ac:dyDescent="0.15">
       <c r="M101" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O101" s="11" t="s">
         <v>30</v>
@@ -4765,7 +5673,7 @@
     </row>
     <row r="102" spans="13:17" x14ac:dyDescent="0.15">
       <c r="M102" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O102" s="11" t="s">
         <v>168</v>
@@ -4773,13 +5681,13 @@
     </row>
     <row r="103" spans="13:17" x14ac:dyDescent="0.15">
       <c r="M103" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="O103" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="O103" s="12"/>
     </row>
     <row r="104" spans="13:17" x14ac:dyDescent="0.15">
       <c r="M104" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O104" s="12" t="s">
         <v>176</v>
@@ -4787,30 +5695,30 @@
     </row>
     <row r="107" spans="13:17" x14ac:dyDescent="0.15">
       <c r="O107" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q107" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="108" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O108" s="11" t="s">
+      <c r="O108" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="Q108" s="11"/>
+      <c r="Q108" s="10"/>
     </row>
     <row r="109" spans="13:17" x14ac:dyDescent="0.15">
       <c r="O109" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="Q109" s="11"/>
+      <c r="Q109" s="12"/>
     </row>
     <row r="110" spans="13:17" x14ac:dyDescent="0.15">
       <c r="O110" s="11" t="s">
         <v>179</v>
       </c>
       <c r="Q110" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="13:17" x14ac:dyDescent="0.15">
@@ -4819,11 +5727,258 @@
       </c>
     </row>
     <row r="112" spans="13:17" x14ac:dyDescent="0.15">
-      <c r="O112" s="11"/>
-    </row>
-    <row r="113" spans="15:15" x14ac:dyDescent="0.15">
+      <c r="O112" s="12"/>
+    </row>
+    <row r="113" spans="5:15" x14ac:dyDescent="0.15">
       <c r="O113" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="116" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="E116" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="117" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I117" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="K117" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="M117" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="O117" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="118" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I118" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="K118" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="M118" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="O118" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="119" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I119" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="K119" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="M119" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="O119" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="120" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I120" s="11"/>
+      <c r="K120" s="11"/>
+      <c r="M120" s="11"/>
+      <c r="O120" s="11"/>
+    </row>
+    <row r="121" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I121" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="K121" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="M121" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="O121" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="122" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F122" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G122" s="3"/>
+      <c r="I122" s="11"/>
+      <c r="K122" s="11"/>
+      <c r="M122" s="11"/>
+      <c r="O122" s="11"/>
+    </row>
+    <row r="123" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F123" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G123" s="3"/>
+      <c r="I123" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="K123" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="M123" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="O123" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="124" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F124" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G124" s="6"/>
+      <c r="I124" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="K124" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="M124" s="12"/>
+      <c r="O124" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="125" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F125" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G125" s="6"/>
+      <c r="I125" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="K125" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="M125" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="O125" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="126" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F126" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G126" s="6"/>
+    </row>
+    <row r="127" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F127" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G127" s="6"/>
+    </row>
+    <row r="128" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F128" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G128" s="6"/>
+    </row>
+    <row r="129" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F129" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G129" s="9"/>
+      <c r="I129" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="K129" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="O129" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F130" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G130" s="9"/>
+      <c r="I130" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="K130" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="O130" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="131" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I131" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="K131" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="O131" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="132" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I132" s="11"/>
+      <c r="K132" s="11"/>
+      <c r="O132" s="11"/>
+    </row>
+    <row r="133" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I133" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="K133" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="O133" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="134" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I134" s="11"/>
+      <c r="K134" s="11"/>
+      <c r="O134" s="11"/>
+    </row>
+    <row r="135" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I135" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K135" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="O135" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="136" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I136" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="K136" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="O136" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="137" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I137" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="K137" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="O137" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="140" spans="6:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K140" s="16" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SR6009_IR fix litter bug about beijing wmtr param set
</commit_message>
<xml_diff>
--- a/doc/水表功能列表.xlsx
+++ b/doc/水表功能列表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="266">
   <si>
     <t>表端</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -871,10 +871,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;&lt;程序升级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.选择升级文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -883,10 +879,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.输入表号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">  &gt; </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -995,10 +987,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>v1.2-ADFE 文件OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>对应老版本的"工程调试"-&gt;"表端操作"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1007,16 +995,88 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">v1.2-ADFE 未开始升级/
+    <t>无应答时，可能处于boot缺包等待状态，需查询缺包数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       无应答时，可能处于boot缺包等待状态，需查询缺包数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Start / Finish / Pkg Wait</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">v1.2 未开始升级/
 升级完成/缺包等待  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无应答时，可能处于boot缺包等待状态，需查询缺包数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">       无应答时，可能处于boot缺包等待状态，需查询缺包数</t>
+    <t xml:space="preserve">    </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;选择升级文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.2     CRC-ADFE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.2     CRC-ADFE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回              确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.添加档案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.删除档案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.清空档案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.升级统计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.查看档案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;批量升级设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;单表升级/批量升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.输入表号/档案设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.单表升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.批量升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级方式      1/2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1261,7 +1321,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1314,7 +1374,7 @@
         <xdr:cNvPr id="5" name="直接箭头连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1367,7 +1427,7 @@
         <xdr:cNvPr id="7" name="直接箭头连接符 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,7 +1480,7 @@
         <xdr:cNvPr id="12" name="直接箭头连接符 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1473,7 +1533,7 @@
         <xdr:cNvPr id="14" name="直接箭头连接符 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1526,7 +1586,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1579,7 +1639,7 @@
         <xdr:cNvPr id="25" name="直接箭头连接符 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1632,7 +1692,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1685,7 +1745,7 @@
         <xdr:cNvPr id="32" name="直接箭头连接符 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1738,7 +1798,7 @@
         <xdr:cNvPr id="34" name="直接箭头连接符 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1791,7 +1851,7 @@
         <xdr:cNvPr id="38" name="直接箭头连接符 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1844,7 +1904,7 @@
         <xdr:cNvPr id="39" name="直接箭头连接符 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1897,7 +1957,7 @@
         <xdr:cNvPr id="58" name="直接箭头连接符 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1950,7 +2010,7 @@
         <xdr:cNvPr id="59" name="直接箭头连接符 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,7 +2063,7 @@
         <xdr:cNvPr id="60" name="直接箭头连接符 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2056,7 +2116,7 @@
         <xdr:cNvPr id="66" name="直接箭头连接符 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2109,7 +2169,7 @@
         <xdr:cNvPr id="20" name="直接箭头连接符 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2162,7 +2222,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2215,7 +2275,7 @@
         <xdr:cNvPr id="26" name="直接箭头连接符 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2268,7 +2328,7 @@
         <xdr:cNvPr id="54" name="直接箭头连接符 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2321,7 +2381,7 @@
         <xdr:cNvPr id="55" name="直接箭头连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2374,7 +2434,7 @@
         <xdr:cNvPr id="57" name="直接箭头连接符 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2427,7 +2487,7 @@
         <xdr:cNvPr id="64" name="直接箭头连接符 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2480,7 +2540,7 @@
         <xdr:cNvPr id="65" name="直接箭头连接符 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2533,7 +2593,7 @@
         <xdr:cNvPr id="67" name="直接箭头连接符 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2586,7 +2646,7 @@
         <xdr:cNvPr id="68" name="直接箭头连接符 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2639,7 +2699,7 @@
         <xdr:cNvPr id="70" name="直接箭头连接符 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2752,7 @@
         <xdr:cNvPr id="71" name="直接箭头连接符 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2745,7 +2805,7 @@
         <xdr:cNvPr id="72" name="直接箭头连接符 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2798,7 +2858,7 @@
         <xdr:cNvPr id="73" name="直接箭头连接符 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000045000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2851,7 +2911,7 @@
         <xdr:cNvPr id="74" name="直接箭头连接符 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000053000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2904,7 +2964,7 @@
         <xdr:cNvPr id="75" name="直接箭头连接符 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2957,7 +3017,7 @@
         <xdr:cNvPr id="76" name="直接箭头连接符 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3010,7 +3070,7 @@
         <xdr:cNvPr id="77" name="直接箭头连接符 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3063,7 +3123,7 @@
         <xdr:cNvPr id="78" name="直接箭头连接符 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3116,7 +3176,7 @@
         <xdr:cNvPr id="79" name="直接箭头连接符 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3169,7 +3229,7 @@
         <xdr:cNvPr id="80" name="直接箭头连接符 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3207,75 +3267,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795618</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>268942</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>33619</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="45" name="直接箭头连接符 44">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3753971" y="20215412"/>
-          <a:ext cx="481853" cy="829236"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>795618</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="52" name="直接箭头连接符 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3283,8 +3290,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3753971" y="21268765"/>
-          <a:ext cx="537882" cy="414617"/>
+          <a:off x="3720353" y="22165236"/>
+          <a:ext cx="504265" cy="1826558"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3314,13 +3321,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1411941</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>145676</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3328,7 +3335,7 @@
         <xdr:cNvPr id="61" name="直接箭头连接符 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3367,13 +3374,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1344705</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>100852</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3381,7 +3388,7 @@
         <xdr:cNvPr id="62" name="直接箭头连接符 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3420,13 +3427,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1535204</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>179292</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3434,7 +3441,7 @@
         <xdr:cNvPr id="69" name="直接箭头连接符 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3473,13 +3480,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>56030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>773206</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>123265</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3487,7 +3494,7 @@
         <xdr:cNvPr id="81" name="直接箭头连接符 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3526,13 +3533,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>78442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>156882</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3540,7 +3547,7 @@
         <xdr:cNvPr id="82" name="直接箭头连接符 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3579,13 +3586,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>201708</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>67237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>134472</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3593,7 +3600,7 @@
         <xdr:cNvPr id="86" name="直接箭头连接符 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3632,13 +3639,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>123265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>78442</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>153</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3646,7 +3653,7 @@
         <xdr:cNvPr id="87" name="直接箭头连接符 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3684,22 +3691,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>336178</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>123267</xdr:rowOff>
+      <xdr:colOff>347382</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>56032</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="88" name="直接箭头连接符 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3707,61 +3714,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3294531" y="21638561"/>
-          <a:ext cx="2812675" cy="1781734"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="89" name="直接箭头连接符 88">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000023000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2846294" y="19543059"/>
-          <a:ext cx="0" cy="694765"/>
+          <a:off x="3305735" y="22546235"/>
+          <a:ext cx="2846295" cy="3406591"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3791,13 +3745,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>941295</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1075765</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3840,13 +3794,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>963706</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>963706</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3884,13 +3838,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1165411</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>56031</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3933,13 +3887,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>403412</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>403413</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3965,6 +3919,324 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>907676</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>268942</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="83" name="直接箭头连接符 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3866029" y="21392029"/>
+          <a:ext cx="414619" cy="874059"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>78439</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="直接箭头连接符 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3059206" y="20585204"/>
+          <a:ext cx="0" cy="437031"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1030941</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1053353</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="直接箭头连接符 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5345206" y="20697265"/>
+          <a:ext cx="22412" cy="425823"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>728382</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="直接箭头连接符 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3686735" y="21941118"/>
+          <a:ext cx="593912" cy="22412"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>773206</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>33619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="95" name="直接箭头连接符 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3731559" y="20204207"/>
+          <a:ext cx="549088" cy="1243852"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>930088</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>201706</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="直接箭头连接符 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3888441" y="19845618"/>
+          <a:ext cx="2151530" cy="1759323"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -4263,10 +4535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S140"/>
+  <dimension ref="A2:S156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O144" sqref="O144"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N120" sqref="N120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4277,7 +4549,7 @@
     <col min="4" max="4" width="4.125" customWidth="1"/>
     <col min="5" max="5" width="13.75" customWidth="1"/>
     <col min="6" max="6" width="4.25" customWidth="1"/>
-    <col min="7" max="7" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="13.75" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="4.125" customWidth="1"/>
@@ -5392,7 +5664,7 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.15">
       <c r="E79" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I79" s="10"/>
       <c r="K79" s="10"/>
@@ -5782,259 +6054,338 @@
         <v>197</v>
       </c>
     </row>
-    <row r="115" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="J115" t="s">
-        <v>249</v>
-      </c>
-    </row>
     <row r="116" spans="5:15" x14ac:dyDescent="0.15">
       <c r="E116" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="117" spans="5:15" x14ac:dyDescent="0.15">
       <c r="I117" s="10" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
       <c r="K117" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="M117" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="O117" s="10" t="s">
-        <v>219</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="I118" s="10" t="s">
-        <v>223</v>
-      </c>
+      <c r="I118" s="10"/>
       <c r="K118" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="M118" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="O118" s="10" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
     </row>
     <row r="119" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="I119" s="11" t="s">
-        <v>220</v>
-      </c>
+      <c r="I119" s="11"/>
       <c r="K119" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="M119" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="O119" s="11" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="I120" s="11"/>
-      <c r="K120" s="11"/>
-      <c r="M120" s="11"/>
-      <c r="O120" s="11"/>
+      <c r="F120" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G120" s="3"/>
+      <c r="I120" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="K120" s="11" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="121" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="I121" s="11" t="s">
-        <v>236</v>
-      </c>
+      <c r="F121" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G121" s="3"/>
+      <c r="I121" s="11"/>
       <c r="K121" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="M121" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="122" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F122" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G122" s="9"/>
+      <c r="I122" s="11"/>
+      <c r="K122" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I123" s="11"/>
+      <c r="K123" s="11"/>
+    </row>
+    <row r="124" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I124" s="12"/>
+      <c r="K124" s="12"/>
+    </row>
+    <row r="125" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="I125" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="K125" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="127" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F127" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G127" s="3"/>
+      <c r="I127" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="128" spans="5:15" x14ac:dyDescent="0.15">
+      <c r="F128" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G128" s="3"/>
+    </row>
+    <row r="129" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F129" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="G129" s="6"/>
+      <c r="J129" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="130" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F130" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G130" s="6"/>
+    </row>
+    <row r="131" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F131" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G131" s="6"/>
+      <c r="I131" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="K131" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="M131" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="O131" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="132" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F132" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G132" s="6"/>
+      <c r="I132" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="K132" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="O121" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="122" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F122" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G122" s="3"/>
-      <c r="I122" s="11"/>
-      <c r="K122" s="11"/>
-      <c r="M122" s="11"/>
-      <c r="O122" s="11"/>
-    </row>
-    <row r="123" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F123" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G123" s="3"/>
-      <c r="I123" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="K123" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="M123" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="O123" s="11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="124" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F124" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G124" s="6"/>
-      <c r="I124" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="K124" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="M124" s="12"/>
-      <c r="O124" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="125" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F125" s="4" t="s">
+      <c r="M132" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="O132" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="133" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F133" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G133" s="6"/>
+      <c r="I133" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="G125" s="6"/>
-      <c r="I125" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="K125" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="M125" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="O125" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="126" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F126" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="G126" s="6"/>
-    </row>
-    <row r="127" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F127" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G127" s="6"/>
-      <c r="I127" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="128" spans="5:15" x14ac:dyDescent="0.15">
-      <c r="F128" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="G128" s="6"/>
-    </row>
-    <row r="129" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="F129" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G129" s="9"/>
-      <c r="I129" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="K129" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="O129" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="130" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="F130" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G130" s="9"/>
-      <c r="I130" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="K130" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="O130" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="131" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="I131" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="K131" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="O131" s="11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="132" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="I132" s="11"/>
-      <c r="K132" s="11"/>
-      <c r="O132" s="11"/>
-    </row>
-    <row r="133" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="I133" s="11" t="s">
-        <v>239</v>
-      </c>
       <c r="K133" s="11" t="s">
-        <v>240</v>
+        <v>218</v>
+      </c>
+      <c r="M133" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="O133" s="11" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F134" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G134" s="9"/>
       <c r="I134" s="11"/>
       <c r="K134" s="11"/>
+      <c r="M134" s="11"/>
       <c r="O134" s="11"/>
     </row>
     <row r="135" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="F135" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G135" s="9"/>
       <c r="I135" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="K135" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="M135" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="O135" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="136" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I136" s="11"/>
+      <c r="K136" s="11"/>
+      <c r="M136" s="11"/>
+      <c r="O136" s="11"/>
+    </row>
+    <row r="137" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I137" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="K137" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="M137" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="O137" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="138" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I138" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="K138" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="M138" s="12"/>
+      <c r="O138" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="K135" s="11" t="s">
+    </row>
+    <row r="139" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I139" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="K139" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="M139" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="O139" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="140" spans="6:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I141" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="143" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I143" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K143" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="O143" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="144" spans="6:15" x14ac:dyDescent="0.15">
+      <c r="I144" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="K144" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="O144" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="145" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I145" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="K145" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="O145" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="146" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I146" s="11"/>
+      <c r="K146" s="11"/>
+      <c r="O146" s="11"/>
+    </row>
+    <row r="147" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I147" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="K147" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="O147" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="148" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I148" s="11"/>
+      <c r="K148" s="11"/>
+      <c r="O148" s="11"/>
+    </row>
+    <row r="149" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I149" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="O135" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="136" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="I136" s="12" t="s">
+      <c r="K149" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="O149" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="150" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I150" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="K150" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="K136" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="O136" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="137" spans="6:15" x14ac:dyDescent="0.15">
-      <c r="I137" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="K137" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="O137" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="140" spans="6:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K140" s="16" t="s">
+      <c r="O150" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="151" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="I151" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="K151" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="O151" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="154" spans="9:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="K154" s="16" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="156" spans="9:15" x14ac:dyDescent="0.15">
+      <c r="K156" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>